<commit_message>
Updated final transistor params
</commit_message>
<xml_diff>
--- a/investigations/ClassEAmps/ClassEFinalTransistors.xlsx
+++ b/investigations/ClassEAmps/ClassEFinalTransistors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jconrad/GitHub/yasdr/investigations/ClassEAmps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571CDBB1-C4EE-6548-8367-D970EEF4E6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDA85D3-E95C-B142-88B7-A21EA8F28039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="8460" windowWidth="23300" windowHeight="7540" xr2:uid="{DDA6A1BA-335A-D741-97D6-B52424E6B1C2}"/>
+    <workbookView xWindow="800" yWindow="2200" windowWidth="23740" windowHeight="10480" xr2:uid="{DDA6A1BA-335A-D741-97D6-B52424E6B1C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{322E84A7-D2A7-D741-94F0-E209E4294BE0}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{322E84A7-D2A7-D741-94F0-E209E4294BE0}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{FDE89B36-CC1A-8A4C-9FC0-9921D17BEB7C}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{FDE89B36-CC1A-8A4C-9FC0-9921D17BEB7C}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{684BE3FB-6921-A74E-AF43-A5FFAD85DFBD}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{684BE3FB-6921-A74E-AF43-A5FFAD85DFBD}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Maximum Ratings</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>(tru)SDX</t>
+  </si>
+  <si>
+    <t>Vgs</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,6 +448,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,19 +767,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C2775E-10D5-7840-BF8F-D23800FEF2A8}">
-  <dimension ref="A2:O9"/>
+  <dimension ref="A2:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="32.6640625" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>13</v>
       </c>
@@ -785,67 +791,71 @@
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="15"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="15"/>
+      <c r="N2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -856,43 +866,46 @@
         <v>60</v>
       </c>
       <c r="D4" s="4">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4">
         <v>0.5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>0.83</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>2.1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>1.2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>0.8</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>24</v>
       </c>
-      <c r="J4" s="7">
+      <c r="K4" s="7">
         <v>17</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L4" s="7">
         <v>7</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>1</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>10</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>10</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -903,39 +916,42 @@
         <v>60</v>
       </c>
       <c r="D5" s="4">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4">
         <v>0.115</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>0.2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>2.1</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>1.2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>0.8</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>20</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="7">
         <v>11</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>4</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="3">
+      <c r="M5" s="8"/>
+      <c r="N5" s="3">
         <v>10</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <v>10</v>
       </c>
-      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -945,36 +961,37 @@
       <c r="C6" s="12">
         <v>30</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="16"/>
+      <c r="E6" s="4">
         <v>4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>1.5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="G6" s="12">
         <v>4</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>50</v>
       </c>
-      <c r="J6" s="7">
+      <c r="K6" s="7">
         <v>40</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L6" s="7">
         <v>1.7</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="9" t="s">
+      <c r="M6" s="8"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -984,40 +1001,43 @@
       <c r="C7" s="12">
         <v>150</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="16">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4">
         <v>1.2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F7" s="12">
+      <c r="G7" s="12">
         <v>3.5</v>
       </c>
-      <c r="G7" s="4">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6">
+      <c r="H7" s="4">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="6">
         <v>55</v>
       </c>
-      <c r="J7" s="7">
+      <c r="K7" s="7">
         <v>8</v>
       </c>
-      <c r="K7" s="7">
+      <c r="L7" s="7">
         <v>1</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="3">
+      <c r="M7" s="8"/>
+      <c r="N7" s="3">
         <v>1.7</v>
       </c>
-      <c r="N7" s="5">
+      <c r="O7" s="5">
         <v>2.6</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1027,42 +1047,43 @@
       <c r="C8" s="12">
         <v>60</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="16"/>
+      <c r="E8" s="4">
         <v>1.2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>1.25</v>
       </c>
-      <c r="F8" s="12">
+      <c r="G8" s="12">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>0.35599999999999998</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>4</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <v>64</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>13</v>
       </c>
-      <c r="K8" s="7">
+      <c r="L8" s="7">
         <v>6.6</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <v>0.67</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="3">
         <v>3.8</v>
       </c>
-      <c r="N8" s="5">
+      <c r="O8" s="5">
         <v>2.8</v>
       </c>
-      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1073,49 +1094,52 @@
         <v>100</v>
       </c>
       <c r="D9" s="4">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4">
         <v>5.6</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>43</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>3</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>0.54</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>10</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>180</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>81</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>15</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M9" s="3">
+      <c r="N9" s="3">
         <v>16</v>
       </c>
-      <c r="N9" s="5">
+      <c r="O9" s="5">
         <v>9.4</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>